<commit_message>
Horaire Simon Tousignant H25
</commit_message>
<xml_diff>
--- a/template/horaire.xlsx
+++ b/template/horaire.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="h:\Users\Simon\Desktop\BD1\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449D1C71-5D82-40F0-8771-5A943D4A64B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CAF4F44-233F-4B1C-ABC6-48835639273A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A6EAA84D-6E98-BB4B-8698-E4F48E48897D}"/>
   </bookViews>
@@ -223,7 +223,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="dd\ mmmm"/>
+    <numFmt numFmtId="164" formatCode="dd\ mmmm"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -256,7 +256,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -594,7 +594,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="C31" sqref="C3:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>